<commit_message>
added rooms and fixed push function
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65c28d79afdf5233/Code/PycharmProjects/s4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremiemarsin/Documents/GitHub/PyVenture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{ECFB69C3-E395-0D47-9C64-056D4CE36F86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D713BB30-59A6-3D4A-84C8-175E28190530}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA976D69-145D-704F-B01F-06AD4B85F05E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27080" yWindow="3080" windowWidth="30340" windowHeight="27080" xr2:uid="{29DF67B7-FB86-004B-8999-80920A454C10}"/>
+    <workbookView xWindow="31480" yWindow="3400" windowWidth="23880" windowHeight="24820" xr2:uid="{29DF67B7-FB86-004B-8999-80920A454C10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>0
 bedroom</t>
@@ -67,6 +67,18 @@
   <si>
     <t>8
 path</t>
+  </si>
+  <si>
+    <t>9
+cave downstairs</t>
+  </si>
+  <si>
+    <t>11
+creek</t>
+  </si>
+  <si>
+    <t>10
+tunnel</t>
   </si>
 </sst>
 </file>
@@ -90,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -215,11 +227,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,7 +292,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -254,16 +303,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -281,6 +339,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>335667</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>835067</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>642321</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Graphic 4" descr="Maximize">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBCD1641-5B40-974B-BAEC-C484648A7EE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="18871069">
+          <a:off x="9987667" y="15382921"/>
+          <a:ext cx="499400" cy="499400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -580,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A537A2-333F-6449-8E5F-3F7E14BD9A95}">
-  <dimension ref="E18:I21"/>
+  <dimension ref="E18:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -595,32 +711,32 @@
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="5:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E18" s="12" t="s">
+    <row r="18" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="5:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E19" s="8"/>
+    <row r="19" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="15"/>
       <c r="F19" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="5:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E20" s="8"/>
+    <row r="20" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="15"/>
       <c r="F20" s="6" t="s">
         <v>2</v>
       </c>
@@ -630,13 +746,24 @@
       <c r="H20" s="10"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="5:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="10"/>
       <c r="F21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -646,5 +773,6 @@
     <mergeCell ref="E18:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added colors to some messages, updated the map
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremiemarsin/Documents/GitHub/PyVenture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremie.marsin.AM-CREATIONS\Git\PyVenture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA976D69-145D-704F-B01F-06AD4B85F05E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CC119F-A12C-423F-9432-F512F96933D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31480" yWindow="3400" windowWidth="23880" windowHeight="24820" xr2:uid="{29DF67B7-FB86-004B-8999-80920A454C10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29DF67B7-FB86-004B-8999-80920A454C10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>0
 bedroom</t>
@@ -79,6 +79,14 @@
   <si>
     <t>10
 tunnel</t>
+  </si>
+  <si>
+    <t>13
+well</t>
+  </si>
+  <si>
+    <t>12
+forest entrance</t>
   </si>
 </sst>
 </file>
@@ -268,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -291,6 +299,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -315,13 +332,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -400,7 +417,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -696,58 +713,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A537A2-333F-6449-8E5F-3F7E14BD9A95}">
-  <dimension ref="E18:K22"/>
+  <dimension ref="D16:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="12" width="15.83203125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="10.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="1"/>
-    <col min="16" max="16" width="10.83203125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="12" width="15.796875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="10.796875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.796875" style="1"/>
+    <col min="16" max="16" width="10.796875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E18" s="8" t="s">
+    <row r="16" spans="5:5" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="19">
+        <v>14</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E19" s="15"/>
+    <row r="19" spans="4:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="18"/>
       <c r="F19" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E20" s="15"/>
+    <row r="20" spans="4:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="18"/>
       <c r="F20" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="11"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E21" s="10"/>
+    <row r="21" spans="4:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="13"/>
       <c r="F21" s="4" t="s">
         <v>3</v>
       </c>
@@ -755,14 +788,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="5:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I22" s="16" t="s">
+    <row r="22" spans="4:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>